<commit_message>
Added defect and attachments
</commit_message>
<xml_diff>
--- a/Setel - Manual Assignment.xlsx
+++ b/Setel - Manual Assignment.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="27795" windowHeight="12855"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="27795" windowHeight="12855" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="66">
   <si>
     <t>Test Case Name:</t>
   </si>
@@ -53,9 +53,6 @@
     <t>App Version</t>
   </si>
   <si>
-    <t>Voucher Top Up</t>
-  </si>
-  <si>
     <t xml:space="preserve">Environment: </t>
   </si>
   <si>
@@ -86,27 +83,6 @@
     <t>2. Login using a valid credentials.</t>
   </si>
   <si>
-    <t>3. Navigate to settings (sandwich icon with 'More' label at the bottom right of the application).</t>
-  </si>
-  <si>
-    <t>4. Go to 'About' page and take screenshot of the 'Version'.</t>
-  </si>
-  <si>
-    <t>1. Navigate to settings (sandwich icon with 'More' label at the bottom right of the application).</t>
-  </si>
-  <si>
-    <t>2. Go to 'Payments' and click 'Payment Method'.</t>
-  </si>
-  <si>
-    <t>3. Click 'Voucher top-up'.</t>
-  </si>
-  <si>
-    <t>4. Enter a valid voucher code.</t>
-  </si>
-  <si>
-    <t>5. Click 'Redeem'.</t>
-  </si>
-  <si>
     <t>P002</t>
   </si>
   <si>
@@ -119,9 +95,6 @@
     <t>Top-up account using an invalid voucher code</t>
   </si>
   <si>
-    <t>4. Enter an invalid voucher code.</t>
-  </si>
-  <si>
     <t>6. Validate the amount that was added in the 'Setel Wallet'</t>
   </si>
   <si>
@@ -135,6 +108,115 @@
   </si>
   <si>
     <t>NotStarted</t>
+  </si>
+  <si>
+    <t>Type:</t>
+  </si>
+  <si>
+    <t>Severity:</t>
+  </si>
+  <si>
+    <t>Status:</t>
+  </si>
+  <si>
+    <t>Component:</t>
+  </si>
+  <si>
+    <t>Action Performed:</t>
+  </si>
+  <si>
+    <t>Expected Result:</t>
+  </si>
+  <si>
+    <t>Actual Result:</t>
+  </si>
+  <si>
+    <t>Build:</t>
+  </si>
+  <si>
+    <t>Device/OS/Browser:</t>
+  </si>
+  <si>
+    <t>Issue Frequency:</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Defect ID: </t>
+  </si>
+  <si>
+    <t>Defect Title:</t>
+  </si>
+  <si>
+    <t>Test Cycle#:</t>
+  </si>
+  <si>
+    <t>Functional</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t>Payments</t>
+  </si>
+  <si>
+    <t>3. Navigate to settings (hamburger icon with 'More' label at the bottom right of the application).</t>
+  </si>
+  <si>
+    <t>2. Go to 'Payments' and tap 'Payment Method'.</t>
+  </si>
+  <si>
+    <t>3. Tap 'Voucher top-up'.</t>
+  </si>
+  <si>
+    <t>5. Tap 'Redeem'.</t>
+  </si>
+  <si>
+    <t>4. Tap 'About'  and take screenshot of the 'Version'.</t>
+  </si>
+  <si>
+    <t>4. Type a valid voucher code.</t>
+  </si>
+  <si>
+    <t>Error response 'This voucher is invalid' should appear below the input field.</t>
+  </si>
+  <si>
+    <t>Pop-up appeared - Top-up failed - Unable to process your voucher top-up. Please try again later.</t>
+  </si>
+  <si>
+    <t>Defect Description</t>
+  </si>
+  <si>
+    <t>Setel 1.91.0(19603)</t>
+  </si>
+  <si>
+    <t>Apple Iphone 13 Pro Max/IOS 15.3.1(19D52)</t>
+  </si>
+  <si>
+    <t>Attachments:</t>
+  </si>
+  <si>
+    <t>Valid Voucher Top Up</t>
+  </si>
+  <si>
+    <t>Invalid Voucher Top Up</t>
+  </si>
+  <si>
+    <t>1. Open Setel app.
+2. Tap on 'More' (hamburger menu icon).
+3. Tap on 'Payment Methods'.
+4. Tap on 'Voucher top-up'.
+5. Type any special character (ie. '-').</t>
+  </si>
+  <si>
+    <t>3/5 - Intermittent</t>
+  </si>
+  <si>
+    <t>Payments - Voucher Top-up - Top-up failed unable to process voucher</t>
   </si>
 </sst>
 </file>
@@ -150,7 +232,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -169,8 +251,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -178,11 +266,89 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -190,16 +356,55 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -212,6 +417,52 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>276225</xdr:colOff>
+          <xdr:row>16</xdr:row>
+          <xdr:rowOff>285750</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>1733550</xdr:colOff>
+          <xdr:row>16</xdr:row>
+          <xdr:rowOff>800100</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2049" name="Object 1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2049"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -503,15 +754,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H173"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="84.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="88" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="50.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.5703125" style="1" customWidth="1"/>
     <col min="7" max="7" width="30.5703125" style="1" customWidth="1"/>
@@ -519,437 +770,437 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="13"/>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="13"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="13"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="4"/>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" s="4"/>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="4"/>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="4"/>
+      <c r="D5" s="13"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="5">
+      <c r="B8" s="6">
         <v>1</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="3" t="s">
+      <c r="E9" s="10"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="6">
+        <v>2</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="5">
-        <v>2</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="3" t="s">
+      <c r="E10" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="3"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="3"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" s="11"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E13" s="3"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" s="10"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="5">
+      <c r="B14" s="6">
         <v>3</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
+      <c r="C14" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="3" t="s">
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" s="11"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="11"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" s="11"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E18" s="11"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="3"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E16" s="3"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E17" s="3"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E18" s="3"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E19" s="3"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="E20" s="2"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D21" s="4"/>
+      <c r="C21" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="13"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D22" s="4"/>
+      <c r="C22" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22" s="13"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C23" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D23" s="4"/>
+      <c r="C23" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" s="13"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D24" s="4"/>
+      <c r="B24" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" s="13"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D26" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="E26" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="F26" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G26" s="5" t="s">
+      <c r="G26" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H26" s="5" t="s">
+      <c r="H26" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="5">
+      <c r="B27" s="6">
         <v>1</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E27" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="G27" s="5"/>
-      <c r="H27" s="5"/>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="3" t="s">
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="6">
+        <v>2</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E28" s="3"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5"/>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="5">
-        <v>2</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D29" s="3" t="s">
+      <c r="E29" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E29" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E30" s="3"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E31" s="3"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E32" s="3"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="5"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="5">
+      <c r="B33" s="6">
         <v>3</v>
       </c>
-      <c r="C33" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="G33" s="5"/>
-      <c r="H33" s="5"/>
+      <c r="C33" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E34" s="3"/>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
-      <c r="H34" s="5"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E35" s="3"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5"/>
-      <c r="H35" s="5"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E35" s="8"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="8"/>
+      <c r="H35" s="8"/>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E36" s="3"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
-      <c r="H36" s="5"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="8"/>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="3" t="s">
+      <c r="B37" s="8"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E37" s="3"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5"/>
-      <c r="H37" s="5"/>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B38" s="5"/>
-      <c r="C38" s="5"/>
-      <c r="D38" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E38" s="3"/>
-      <c r="F38" s="5"/>
-      <c r="G38" s="5"/>
-      <c r="H38" s="5"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="7"/>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="E39" s="2"/>
@@ -1357,18 +1608,220 @@
       <c r="E173" s="2"/>
     </row>
   </sheetData>
+  <mergeCells count="44">
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="B14:B19"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="C14:C19"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="H10:H13"/>
+    <mergeCell ref="H14:H19"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="E10:E13"/>
+    <mergeCell ref="E14:E19"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="F10:F13"/>
+    <mergeCell ref="F14:F19"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="G10:G13"/>
+    <mergeCell ref="G14:G19"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="G29:G32"/>
+    <mergeCell ref="G33:G38"/>
+    <mergeCell ref="H27:H28"/>
+    <mergeCell ref="H29:H32"/>
+    <mergeCell ref="H33:H38"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="E29:E32"/>
+    <mergeCell ref="E33:E38"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="F29:F32"/>
+    <mergeCell ref="F33:F38"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="B29:B32"/>
+    <mergeCell ref="B33:B38"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="C29:C32"/>
+    <mergeCell ref="C33:C38"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:C17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="21.5703125" customWidth="1"/>
+    <col min="3" max="3" width="99.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="20"/>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="B11" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" s="16"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B9:C9"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <oleObjects>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <oleObject progId="Packager Shell Object" shapeId="2049" r:id="rId4">
+          <objectPr defaultSize="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>276225</xdr:colOff>
+                <xdr:row>16</xdr:row>
+                <xdr:rowOff>285750</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>1733550</xdr:colOff>
+                <xdr:row>16</xdr:row>
+                <xdr:rowOff>800100</xdr:rowOff>
+              </to>
+            </anchor>
+          </objectPr>
+        </oleObject>
+      </mc:Choice>
+      <mc:Fallback>
+        <oleObject progId="Packager Shell Object" shapeId="2049" r:id="rId4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+  </oleObjects>
 </worksheet>
 </file>
</xml_diff>